<commit_message>
Spring Break Monday and Tuesday work
</commit_message>
<xml_diff>
--- a/24-25Year/Spring25/DES-315/des-315-card-game/CardGameInterface.xlsx
+++ b/24-25Year/Spring25/DES-315/des-315-card-game/CardGameInterface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KingLoui1221\Documents\DIT Stuff\DITRepo\DITWork\24-25Year\Spring25\DES-315\des-315-card-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7B3B24-23B1-4FDF-8A87-5EE50FCCAF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E26945A-C9AF-461A-96B9-24FE93E7FC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2252,8 +2252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -2633,10 +2633,10 @@
     <row r="35" spans="1:5" s="2" customFormat="1" ht="31.5">
       <c r="A35" s="21">
         <f t="shared" ref="A35:A37" si="7">IF(LEFT(B35,2)="No",-0.1,IF(LEFT(B35,7)="Partial",0.01,IF(LEFT(B35,4)="Full",0.03,"n/a")))</f>
-        <v>-0.1</v>
+        <v>0.01</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" s="39" t="s">
         <v>24</v>

</xml_diff>